<commit_message>
generated outputs from the power distribution and flight controller boards
</commit_message>
<xml_diff>
--- a/cad/pcb/altium/outputs/power/BOM/Bill of Materials-power_dist.xlsx
+++ b/cad/pcb/altium/outputs/power/BOM/Bill of Materials-power_dist.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0BFBB8C4-A03B-4E67-BE57-668F3D8F119C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{896D711F-5A2A-4605-AFE6-47DFACF91C69}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10215" xr2:uid="{5582BA6C-BB24-45A2-A89B-885B1701B853}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7848" xr2:uid="{E14A1260-510A-4482-B7BF-ECBEF9079167}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-power_dist" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -264,7 +264,7 @@
     <t>H1, H2, H3, H4</t>
   </si>
   <si>
-    <t>6mm Mount Hole</t>
+    <t>4mm Mount Hole</t>
   </si>
   <si>
     <t>22 uH</t>
@@ -1102,17 +1102,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02B62765-5A3D-43AB-A2B4-F5134892205A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAD3CC2E-4F04-4061-83EC-54A99B783FAE}">
   <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="9" width="14.42578125" customWidth="1"/>
+    <col min="1" max="9" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -1170,7 +1170,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>37</v>
       </c>
@@ -1286,7 +1286,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>43</v>
       </c>
@@ -1315,7 +1315,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>47</v>
       </c>
@@ -1344,7 +1344,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>53</v>
       </c>
@@ -1373,7 +1373,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>59</v>
       </c>
@@ -1402,7 +1402,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>64</v>
       </c>
@@ -1431,7 +1431,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>71</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>77</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>80</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>87</v>
       </c>
@@ -1547,7 +1547,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>91</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>95</v>
       </c>
@@ -1605,7 +1605,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>90</v>
       </c>
@@ -1634,7 +1634,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>100</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>107</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>114</v>
       </c>
@@ -1721,7 +1721,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>121</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>127</v>
       </c>
@@ -1779,7 +1779,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>132</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>137</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>142</v>
       </c>
@@ -1866,7 +1866,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>145</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>151</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>157</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>162</v>
       </c>
@@ -1982,7 +1982,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>167</v>
       </c>
@@ -2011,7 +2011,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>170</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>177</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>180</v>
       </c>
@@ -2098,7 +2098,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>183</v>
       </c>
@@ -2127,7 +2127,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>188</v>
       </c>
@@ -2156,7 +2156,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>145</v>
       </c>
@@ -2185,7 +2185,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>195</v>
       </c>
@@ -2214,7 +2214,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>202</v>
       </c>
@@ -2243,7 +2243,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>209</v>
       </c>
@@ -2272,7 +2272,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>215</v>
       </c>
@@ -2301,7 +2301,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>221</v>
       </c>
@@ -2332,90 +2332,90 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" tooltip="Manufacturer" display="'C3216X5R1E106M085AC" xr:uid="{05ACFEE0-F65F-428A-AF3B-96A92F6EABD8}"/>
-    <hyperlink ref="I2" r:id="rId2" tooltip="Supplier" display="'445-14678-6-ND" xr:uid="{D9EA560D-E604-4D3D-9FA7-06432D998ABF}"/>
-    <hyperlink ref="F3" r:id="rId3" tooltip="Manufacturer" display="'CL10B333KA8WPNC" xr:uid="{5A0451F0-2238-4E32-89F7-BDBBD00A9EB7}"/>
-    <hyperlink ref="I3" r:id="rId4" tooltip="Supplier" display="'1276-6675-6-ND" xr:uid="{40489DD1-FFC8-4F94-AE81-CA4AF4F5192A}"/>
-    <hyperlink ref="F4" r:id="rId5" tooltip="Manufacturer" display="'GRM21BR61E106KA73L" xr:uid="{D47BA3A4-223F-4B54-B7DE-EC855C831DC5}"/>
-    <hyperlink ref="I4" r:id="rId6" tooltip="Supplier" display="'490-5523-6-ND" xr:uid="{48D57539-4365-4444-928B-8A7218A22954}"/>
-    <hyperlink ref="F5" r:id="rId7" tooltip="Manufacturer" display="'EEE-FC1A101P, EEE-FC1E101P" xr:uid="{E1C00F93-8A0E-4A51-A5D7-DE48DEA4B81D}"/>
-    <hyperlink ref="I5" r:id="rId8" tooltip="Supplier" display="'PCE3989DKR-ND, PCE4003DKR-ND" xr:uid="{11C2FC0C-A9A9-42D5-B403-CA5C4154BA78}"/>
-    <hyperlink ref="F6" r:id="rId9" tooltip="Manufacturer" display="'CC0603MRX7R9BB471" xr:uid="{288AC797-310B-42CE-AEE4-BC2A155E874F}"/>
-    <hyperlink ref="I6" r:id="rId10" tooltip="Supplier" display="'311-3377-6-ND" xr:uid="{2078A2A6-3E0F-4212-9BB6-264A8366CF78}"/>
-    <hyperlink ref="F7" tooltip="Manufacturer" display="'" xr:uid="{D7F3302A-4292-453C-8EA5-1F8E1CD910F2}"/>
-    <hyperlink ref="I7" tooltip="Supplier" display="'" xr:uid="{3F3E95AE-A0B3-4EE9-A934-AA3DF611AEB1}"/>
-    <hyperlink ref="F8" r:id="rId11" tooltip="Manufacturer" display="'C0603C103M3RACTU" xr:uid="{07A48BE6-5910-4899-AAE8-FB9A12CE234D}"/>
-    <hyperlink ref="I8" r:id="rId12" tooltip="Supplier" display="'399-8989-6-ND" xr:uid="{9A6E2F90-BD5B-4123-9C85-08922983EA78}"/>
-    <hyperlink ref="F9" r:id="rId13" tooltip="Manufacturer" display="'885012206064" xr:uid="{2D5ED569-2B75-4CCB-B088-ED1BF3597141}"/>
-    <hyperlink ref="I9" r:id="rId14" tooltip="Supplier" display="'732-7982-6-ND" xr:uid="{D1E0B5FA-1F50-4C95-89DC-375D8E93CFEF}"/>
-    <hyperlink ref="F10" tooltip="Manufacturer" display="'" xr:uid="{ED7102A4-B8C5-4601-B5EC-C00911AF969E}"/>
-    <hyperlink ref="I10" tooltip="Supplier" display="'" xr:uid="{7049ED93-19E8-4EF4-9749-85A1D11A40BD}"/>
-    <hyperlink ref="F11" r:id="rId15" tooltip="Manufacturer" display="'MBRS330T3G" xr:uid="{7C0D18F1-53D5-4BC6-A58D-FF3A49959BE2}"/>
-    <hyperlink ref="I11" r:id="rId16" tooltip="Supplier" display="'MBRS330T3GOSDKR-ND" xr:uid="{2B182F1C-2290-4782-AE12-CB192A6E170A}"/>
-    <hyperlink ref="F12" r:id="rId17" tooltip="Manufacturer" display="'Q62702P5179" xr:uid="{BC9DA458-DD1C-407C-BB33-A37308FC9754}"/>
-    <hyperlink ref="I12" r:id="rId18" tooltip="Supplier" display="'475-1410-1-ND" xr:uid="{76BE49BC-7D7E-4A67-B50F-61C61EB2EBCA}"/>
-    <hyperlink ref="F13" tooltip="Manufacturer" display="'" xr:uid="{4ABCA0E1-CEC4-4861-89FA-07608D2861D1}"/>
-    <hyperlink ref="I13" tooltip="Supplier" display="'" xr:uid="{13D6C4E9-E8EA-4C0F-AE01-54298DC5CF80}"/>
-    <hyperlink ref="F14" r:id="rId19" tooltip="Manufacturer" display="'SRR1210-220M" xr:uid="{F12DE791-FB5A-4B6E-8A43-B77D4AB427EF}"/>
-    <hyperlink ref="I14" r:id="rId20" tooltip="Supplier" display="'SRR1210-220MDKR-ND" xr:uid="{D6039F1B-2B31-4B43-BE7D-182DB6FA72EC}"/>
-    <hyperlink ref="F15" tooltip="Manufacturer" display="'" xr:uid="{8F7D1ED3-3EF8-4272-858C-5815DD4707C2}"/>
-    <hyperlink ref="I15" tooltip="Supplier" display="'" xr:uid="{30733DA6-95E5-42FD-BA1F-E63BDFA50E22}"/>
-    <hyperlink ref="F16" tooltip="Manufacturer" display="'" xr:uid="{CF27B2E4-1E65-4287-825C-CB6B043F2F5A}"/>
-    <hyperlink ref="I16" tooltip="Supplier" display="'" xr:uid="{68497F60-9D8B-4A87-BDBF-0E2D835CB5F7}"/>
-    <hyperlink ref="F17" tooltip="Manufacturer" display="'" xr:uid="{67C8A246-7579-4C7E-BB4A-E432ADACF0AB}"/>
-    <hyperlink ref="I17" tooltip="Supplier" display="'" xr:uid="{0C6CE1F0-CE1D-4433-BE46-73423158DC9E}"/>
-    <hyperlink ref="F18" tooltip="Manufacturer" display="'" xr:uid="{AAB85A32-D063-4B08-8B0D-B53A4EAFC5CC}"/>
-    <hyperlink ref="I18" tooltip="Supplier" display="'" xr:uid="{3D5C0C65-8F0F-477D-BE58-4004B4A69102}"/>
-    <hyperlink ref="F19" r:id="rId21" tooltip="Manufacturer" display="'2N7002K-T1-E3" xr:uid="{A87E0225-6A33-441E-926A-6FBBA224217F}"/>
-    <hyperlink ref="I19" r:id="rId22" tooltip="Supplier" display="'2N7002K-T1-E3DKR-ND" xr:uid="{6AA8B06B-7A48-42D9-82E8-7480E04BFE33}"/>
-    <hyperlink ref="F20" r:id="rId23" tooltip="Manufacturer" display="'SQJQ900E-T1_GE3" xr:uid="{7AD7750D-CBA4-4216-A9AE-136E1DBDE311}"/>
-    <hyperlink ref="I20" r:id="rId24" tooltip="Supplier" display="'SQJQ900E-T1_GE3DKR-ND" xr:uid="{D07FCE29-261A-47FA-AF2F-0889EC7BFBF5}"/>
-    <hyperlink ref="F21" r:id="rId25" tooltip="Manufacturer" display="'ESR03EZPJ100" xr:uid="{8B4AAFC2-0526-4A1F-B352-B08AFC49AD1F}"/>
-    <hyperlink ref="I21" r:id="rId26" tooltip="Supplier" display="'RHM10DDKR-ND" xr:uid="{645FB328-6437-4765-94AE-9BD7FFECD34E}"/>
-    <hyperlink ref="F22" r:id="rId27" tooltip="Manufacturer" display="'ERJ3EKF-2002V" xr:uid="{80BB4E13-B067-41E8-9022-C9F482393F46}"/>
-    <hyperlink ref="I22" r:id="rId28" tooltip="Supplier" display="'P20.0KHDKR-ND" xr:uid="{041B43F1-28A3-481D-9537-4C487D1EEC30}"/>
-    <hyperlink ref="F23" r:id="rId29" tooltip="Manufacturer" display="'ERJ-3EKF3831V" xr:uid="{28657285-29F3-4DAE-B037-1F98BEF481A8}"/>
-    <hyperlink ref="I23" r:id="rId30" tooltip="Supplier" display="'P3.83KHDKR-ND" xr:uid="{388D38B9-16E8-4350-956C-850E145EFE0E}"/>
-    <hyperlink ref="F24" r:id="rId31" tooltip="Manufacturer" display="'RC0603FR-07422RL" xr:uid="{1D6A2858-8307-4417-862C-288311D10A3C}"/>
-    <hyperlink ref="I24" r:id="rId32" tooltip="Supplier" display="'311-422HRCT-ND" xr:uid="{EEFF5A73-99DF-4C3D-AB95-16572F516070}"/>
-    <hyperlink ref="F25" tooltip="Manufacturer" display="'" xr:uid="{3EB37D87-4A62-4DC0-B4FF-FA733D9053A1}"/>
-    <hyperlink ref="I25" tooltip="Supplier" display="'" xr:uid="{6BAE93E0-9811-4364-AE84-DA7F9CE29C89}"/>
-    <hyperlink ref="F26" tooltip="Manufacturer" display="'" xr:uid="{F0441F94-E7A0-4C3E-BCF1-7CF03B51E244}"/>
-    <hyperlink ref="I26" tooltip="Supplier" display="'" xr:uid="{5BB42519-9E56-43BA-9E4A-6CD607B9CD0A}"/>
-    <hyperlink ref="F27" r:id="rId33" tooltip="Manufacturer" display="'ERJ-3GEY0R00V" xr:uid="{8F4014EA-106F-48D1-ADAF-BC072B6E17DA}"/>
-    <hyperlink ref="I27" r:id="rId34" tooltip="Supplier" display="'P0.0GDKR-ND" xr:uid="{AEC1F307-A955-4F8C-A3E5-1C2ED0B391D0}"/>
-    <hyperlink ref="F28" r:id="rId35" tooltip="Manufacturer" display="'ERJ-6ENF1874V" xr:uid="{DA2DFC53-AE45-4C25-8262-B206F9DCF3F2}"/>
-    <hyperlink ref="I28" r:id="rId36" tooltip="Supplier" display="'P1.87BTDKR-ND" xr:uid="{B16C237E-9706-4B6B-B1B9-15BD3600CEC1}"/>
-    <hyperlink ref="F29" r:id="rId37" tooltip="Manufacturer" display="'ERJ-6ENF4532V" xr:uid="{4A332102-EC58-4BC4-BD66-B2D465B2671D}"/>
-    <hyperlink ref="I29" r:id="rId38" tooltip="Supplier" display="'P45.3KCDKR-ND" xr:uid="{EAEA232B-14A4-4B90-8029-9F5B51B63AD2}"/>
-    <hyperlink ref="F30" r:id="rId39" tooltip="Manufacturer" display="'CRCW080554K9FKEA" xr:uid="{AFE4453A-D410-40CE-A3DC-09A32817FE54}"/>
-    <hyperlink ref="I30" r:id="rId40" tooltip="Supplier" display="'541-54.9KCDKR-ND" xr:uid="{9D170234-ED5E-4F3B-997B-E009B590FA8A}"/>
-    <hyperlink ref="F31" tooltip="Manufacturer" display="'" xr:uid="{CEA26F7B-8A6A-47B9-849E-5DC823E6D21A}"/>
-    <hyperlink ref="I31" tooltip="Supplier" display="'" xr:uid="{AE94BAC0-2043-4893-8FC8-5D1079A1716B}"/>
-    <hyperlink ref="F32" r:id="rId41" tooltip="Manufacturer" display="'WSLF2512L3000FEA" xr:uid="{768F7F65-875A-4A7E-BE34-FD51B3A7323F}"/>
-    <hyperlink ref="I32" r:id="rId42" tooltip="Supplier" display="'541-3123-6-ND" xr:uid="{E03E5D22-509A-4FBB-9000-86ED80D1632C}"/>
-    <hyperlink ref="F33" tooltip="Manufacturer" display="'" xr:uid="{58845270-F21E-4655-B297-3184B9558A7F}"/>
-    <hyperlink ref="I33" tooltip="Supplier" display="'" xr:uid="{05C861BD-DF04-436E-AC2F-FCDC043620EE}"/>
-    <hyperlink ref="F34" tooltip="Manufacturer" display="'" xr:uid="{564F8848-61DF-4CB2-AFD4-2E8437D869E6}"/>
-    <hyperlink ref="I34" tooltip="Supplier" display="'" xr:uid="{6C1501DE-B985-4214-BECE-F1EA69BD2BAD}"/>
-    <hyperlink ref="F35" r:id="rId43" tooltip="Manufacturer" display="'RC0603FR-076K34L" xr:uid="{161963ED-BBE7-4034-AAC2-C8F2755F8BED}"/>
-    <hyperlink ref="I35" r:id="rId44" tooltip="Supplier" display="'311-6.34KHRDKR-ND" xr:uid="{FB1DC86B-C1BA-480C-9850-24CBB404463F}"/>
-    <hyperlink ref="F36" r:id="rId45" tooltip="Manufacturer" display="'RMCF0603FT698R" xr:uid="{CD296080-0B8D-47FB-A483-5A363E576126}"/>
-    <hyperlink ref="I36" r:id="rId46" tooltip="Supplier" display="'RMCF0603FT698RDKR-ND" xr:uid="{F13AA692-2CA8-447B-B72A-109993C3C486}"/>
-    <hyperlink ref="F37" tooltip="Manufacturer" display="'" xr:uid="{40A977AF-279B-4FD1-BF7D-9EFBE11641DD}"/>
-    <hyperlink ref="I37" tooltip="Supplier" display="'" xr:uid="{DFF964D7-8E68-4C64-A088-FB37FA5AEABD}"/>
-    <hyperlink ref="F38" r:id="rId47" tooltip="Manufacturer" display="'SS312SAH4-R" xr:uid="{5D3E877B-AEE9-4CE8-A65F-DF43659697CA}"/>
-    <hyperlink ref="I38" r:id="rId48" tooltip="Supplier" display="'360-2924-1-ND" xr:uid="{02652ED1-087C-4360-90BF-472EDF7AB27D}"/>
-    <hyperlink ref="F39" r:id="rId49" tooltip="Manufacturer" display="'TPS54383PWPR" xr:uid="{EA76FFE6-36F5-475E-B6F4-72CB3A843659}"/>
-    <hyperlink ref="I39" r:id="rId50" tooltip="Supplier" display="'296-23087-6-ND" xr:uid="{CD157B6E-DB67-4BCB-AED8-DA6B4D8669C5}"/>
-    <hyperlink ref="F40" r:id="rId51" tooltip="Manufacturer" display="'INA199B2DCKR" xr:uid="{49CC6212-A67A-4DD2-9A5C-8AFB4312EF5B}"/>
-    <hyperlink ref="I40" r:id="rId52" tooltip="Supplier" display="'INA199B2DCKR-ND" xr:uid="{E5E3FBEF-529A-4D2C-8759-23335B60B34A}"/>
-    <hyperlink ref="F41" r:id="rId53" tooltip="Manufacturer" display="'TPS3705-33D" xr:uid="{2C3C621E-2B15-49C1-9B6E-840A15912ED3}"/>
-    <hyperlink ref="I41" r:id="rId54" tooltip="Supplier" display="'296-2623-5-ND" xr:uid="{5B9E5A33-B2E6-416C-8CC0-08E0690D0375}"/>
-    <hyperlink ref="F42" r:id="rId55" tooltip="Manufacturer" display="'LTC4365CTS8#TRMPBF" xr:uid="{604828A0-3C30-46F1-ACAA-E2E20945510D}"/>
-    <hyperlink ref="I42" r:id="rId56" tooltip="Supplier" display="'LTC4365CTS8#TRMPBFDKR-ND" xr:uid="{272F3A6C-FF57-4C7F-8DB3-96E5C72D69AB}"/>
+    <hyperlink ref="F2" r:id="rId1" tooltip="Manufacturer" display="'C3216X5R1E106M085AC" xr:uid="{B7804C26-0658-48CE-B12E-D84462408B05}"/>
+    <hyperlink ref="I2" r:id="rId2" tooltip="Supplier" display="'445-14678-6-ND" xr:uid="{A46B9FAB-494D-4595-B31B-C808CE29546C}"/>
+    <hyperlink ref="F3" r:id="rId3" tooltip="Manufacturer" display="'CL10B333KA8WPNC" xr:uid="{FE981C90-4471-4E13-A93B-59ECD0E8DBC1}"/>
+    <hyperlink ref="I3" r:id="rId4" tooltip="Supplier" display="'1276-6675-6-ND" xr:uid="{046DC2BC-3DE1-42E6-BE99-8DD1E956905F}"/>
+    <hyperlink ref="F4" r:id="rId5" tooltip="Manufacturer" display="'GRM21BR61E106KA73L" xr:uid="{A969ABFF-DE49-437E-9B9A-ACF513740606}"/>
+    <hyperlink ref="I4" r:id="rId6" tooltip="Supplier" display="'490-5523-6-ND" xr:uid="{A5980AAA-8655-4449-9C8B-F8CE2DB2FE13}"/>
+    <hyperlink ref="F5" r:id="rId7" tooltip="Manufacturer" display="'EEE-FC1A101P, EEE-FC1E101P" xr:uid="{3B657B5F-C6E6-47D1-8CA2-3F4912005C0C}"/>
+    <hyperlink ref="I5" r:id="rId8" tooltip="Supplier" display="'PCE3989DKR-ND, PCE4003DKR-ND" xr:uid="{304FF7A7-3397-4FC6-A42B-BB1A75A8CE2A}"/>
+    <hyperlink ref="F6" r:id="rId9" tooltip="Manufacturer" display="'CC0603MRX7R9BB471" xr:uid="{DB59107D-8C96-48CE-BE9D-D31BBC3A914A}"/>
+    <hyperlink ref="I6" r:id="rId10" tooltip="Supplier" display="'311-3377-6-ND" xr:uid="{2F99FA5A-E12A-4BA3-A606-FD4DD4FD4DD5}"/>
+    <hyperlink ref="F7" tooltip="Manufacturer" display="'" xr:uid="{544DA009-EF1E-461C-B3B5-10D4E1B7158A}"/>
+    <hyperlink ref="I7" tooltip="Supplier" display="'" xr:uid="{2402FEE3-FC2B-42D4-BEB9-D5C139544A1D}"/>
+    <hyperlink ref="F8" r:id="rId11" tooltip="Manufacturer" display="'C0603C103M3RACTU" xr:uid="{12FB7199-B963-4976-BA1B-1D604DD4A1B3}"/>
+    <hyperlink ref="I8" r:id="rId12" tooltip="Supplier" display="'399-8989-6-ND" xr:uid="{9D4DDEB7-14E3-4A69-927F-7F227F63BA11}"/>
+    <hyperlink ref="F9" r:id="rId13" tooltip="Manufacturer" display="'885012206064" xr:uid="{E4068237-53BD-4A37-8011-73B0295B8130}"/>
+    <hyperlink ref="I9" r:id="rId14" tooltip="Supplier" display="'732-7982-6-ND" xr:uid="{20274E47-2E10-4920-9A2A-4FE4BD4F194C}"/>
+    <hyperlink ref="F10" tooltip="Manufacturer" display="'" xr:uid="{26DDE7FF-190F-48D2-8914-25853C8AB95C}"/>
+    <hyperlink ref="I10" tooltip="Supplier" display="'" xr:uid="{EF131AEC-0C50-45B6-84CF-E50476631B86}"/>
+    <hyperlink ref="F11" r:id="rId15" tooltip="Manufacturer" display="'MBRS330T3G" xr:uid="{8E165E28-ADB0-4895-A1A5-A6797D27F8B7}"/>
+    <hyperlink ref="I11" r:id="rId16" tooltip="Supplier" display="'MBRS330T3GOSDKR-ND" xr:uid="{176C9314-F710-474C-B590-B08C86DA992B}"/>
+    <hyperlink ref="F12" r:id="rId17" tooltip="Manufacturer" display="'Q62702P5179" xr:uid="{80B4C58E-F603-413C-ACD7-702F6B188993}"/>
+    <hyperlink ref="I12" r:id="rId18" tooltip="Supplier" display="'475-1410-1-ND" xr:uid="{36DFED3A-782A-4ADC-A325-248263992E89}"/>
+    <hyperlink ref="F13" tooltip="Manufacturer" display="'" xr:uid="{E38549EF-C3FB-4DEC-92FD-B3435360E924}"/>
+    <hyperlink ref="I13" tooltip="Supplier" display="'" xr:uid="{16C2E1CE-21FC-4F76-A8F0-30F252C73FE7}"/>
+    <hyperlink ref="F14" r:id="rId19" tooltip="Manufacturer" display="'SRR1210-220M" xr:uid="{65DB5FB4-7DEE-400C-BD85-D49C1F4FCA23}"/>
+    <hyperlink ref="I14" r:id="rId20" tooltip="Supplier" display="'SRR1210-220MDKR-ND" xr:uid="{A5EE3F09-8135-4818-8B0C-D438EABD19E6}"/>
+    <hyperlink ref="F15" tooltip="Manufacturer" display="'" xr:uid="{2AD8A083-053C-4F37-BB55-607852932979}"/>
+    <hyperlink ref="I15" tooltip="Supplier" display="'" xr:uid="{A3376224-DF8D-4049-BF0A-096DACF31E48}"/>
+    <hyperlink ref="F16" tooltip="Manufacturer" display="'" xr:uid="{23CC5B52-71B9-485B-9D07-AABE81E1846C}"/>
+    <hyperlink ref="I16" tooltip="Supplier" display="'" xr:uid="{FBC0D6D6-ED3C-4BE2-9CBB-A510B0EBA76C}"/>
+    <hyperlink ref="F17" tooltip="Manufacturer" display="'" xr:uid="{03126CB4-01B9-45BB-B124-6B7C5C8C3D45}"/>
+    <hyperlink ref="I17" tooltip="Supplier" display="'" xr:uid="{3811E853-F12B-434A-8292-87E7ED0C3E72}"/>
+    <hyperlink ref="F18" tooltip="Manufacturer" display="'" xr:uid="{90977E4E-56E7-4847-B9AD-81716A68A01C}"/>
+    <hyperlink ref="I18" tooltip="Supplier" display="'" xr:uid="{06F1EBD7-679A-49C4-96E2-AC48917C3BAE}"/>
+    <hyperlink ref="F19" r:id="rId21" tooltip="Manufacturer" display="'2N7002K-T1-E3" xr:uid="{D3C1B1E4-6825-4D40-8C29-49F96BF5AAD1}"/>
+    <hyperlink ref="I19" r:id="rId22" tooltip="Supplier" display="'2N7002K-T1-E3DKR-ND" xr:uid="{ACEE6A5E-2AE9-471D-93A7-B4F30D76D6CF}"/>
+    <hyperlink ref="F20" r:id="rId23" tooltip="Manufacturer" display="'SQJQ900E-T1_GE3" xr:uid="{6F0FDCA0-3DAC-4232-A7D8-05091CFEEB40}"/>
+    <hyperlink ref="I20" r:id="rId24" tooltip="Supplier" display="'SQJQ900E-T1_GE3DKR-ND" xr:uid="{C28A5C1D-A94C-4DB4-81FA-9525423F919D}"/>
+    <hyperlink ref="F21" r:id="rId25" tooltip="Manufacturer" display="'ESR03EZPJ100" xr:uid="{27A4FED8-A92A-44E5-9A6B-4C2A3C3F08BD}"/>
+    <hyperlink ref="I21" r:id="rId26" tooltip="Supplier" display="'RHM10DDKR-ND" xr:uid="{F9F25B3E-6DD3-433E-AAC7-508DA4ECE5FF}"/>
+    <hyperlink ref="F22" r:id="rId27" tooltip="Manufacturer" display="'ERJ3EKF-2002V" xr:uid="{14C8E8AD-18D1-4282-A177-022E9CD5F2C6}"/>
+    <hyperlink ref="I22" r:id="rId28" tooltip="Supplier" display="'P20.0KHDKR-ND" xr:uid="{855DA6A2-8B4C-46A9-BB1B-F11A63F29F24}"/>
+    <hyperlink ref="F23" r:id="rId29" tooltip="Manufacturer" display="'ERJ-3EKF3831V" xr:uid="{C72E92D1-DF0E-4244-8E99-6AD41E3B511E}"/>
+    <hyperlink ref="I23" r:id="rId30" tooltip="Supplier" display="'P3.83KHDKR-ND" xr:uid="{300DFDC2-451C-453E-A810-99289294A72C}"/>
+    <hyperlink ref="F24" r:id="rId31" tooltip="Manufacturer" display="'RC0603FR-07422RL" xr:uid="{B9F1F32E-6E11-4A10-95D1-DA27EEF0B966}"/>
+    <hyperlink ref="I24" r:id="rId32" tooltip="Supplier" display="'311-422HRCT-ND" xr:uid="{BE2ADD3E-7AA2-4EF4-8610-0A9666113B08}"/>
+    <hyperlink ref="F25" tooltip="Manufacturer" display="'" xr:uid="{BC67B5BE-288D-47D4-9FDC-24D0D3F37589}"/>
+    <hyperlink ref="I25" tooltip="Supplier" display="'" xr:uid="{DD23AF9C-F8CD-4CB6-A9E6-93063E41E567}"/>
+    <hyperlink ref="F26" tooltip="Manufacturer" display="'" xr:uid="{B7A2BE80-3950-47FF-80ED-A1B130D42FA7}"/>
+    <hyperlink ref="I26" tooltip="Supplier" display="'" xr:uid="{02D55C81-4153-41A1-A39C-035EB1F3CBE2}"/>
+    <hyperlink ref="F27" r:id="rId33" tooltip="Manufacturer" display="'ERJ-3GEY0R00V" xr:uid="{FDB6C4E7-6EA5-4C83-AD74-06C3D280E08F}"/>
+    <hyperlink ref="I27" r:id="rId34" tooltip="Supplier" display="'P0.0GDKR-ND" xr:uid="{8E328691-0FD7-4311-8F7D-7F443D171531}"/>
+    <hyperlink ref="F28" r:id="rId35" tooltip="Manufacturer" display="'ERJ-6ENF1874V" xr:uid="{C1BE0D9C-97EC-4FDD-97C1-1C225C1AB4CE}"/>
+    <hyperlink ref="I28" r:id="rId36" tooltip="Supplier" display="'P1.87BTDKR-ND" xr:uid="{8D1044CD-0AA2-4343-97C4-5B8FB5ADD76D}"/>
+    <hyperlink ref="F29" r:id="rId37" tooltip="Manufacturer" display="'ERJ-6ENF4532V" xr:uid="{B5C58265-3FC6-427B-A49E-CF6BD366FCDA}"/>
+    <hyperlink ref="I29" r:id="rId38" tooltip="Supplier" display="'P45.3KCDKR-ND" xr:uid="{BBF512C3-AACD-4273-A9A8-65FCBA3FC176}"/>
+    <hyperlink ref="F30" r:id="rId39" tooltip="Manufacturer" display="'CRCW080554K9FKEA" xr:uid="{5FAD8C04-1548-4D11-A34F-03192ACE46F3}"/>
+    <hyperlink ref="I30" r:id="rId40" tooltip="Supplier" display="'541-54.9KCDKR-ND" xr:uid="{4E71D2BF-A68B-44FF-A525-88686B9DF88C}"/>
+    <hyperlink ref="F31" tooltip="Manufacturer" display="'" xr:uid="{331E06CF-2D7E-4AA9-A799-3C32CC134BA4}"/>
+    <hyperlink ref="I31" tooltip="Supplier" display="'" xr:uid="{00F75D00-5BA0-4C0D-BA4E-9DC982C5CF7E}"/>
+    <hyperlink ref="F32" r:id="rId41" tooltip="Manufacturer" display="'WSLF2512L3000FEA" xr:uid="{88BD883D-AE30-43A8-A897-75033E675536}"/>
+    <hyperlink ref="I32" r:id="rId42" tooltip="Supplier" display="'541-3123-6-ND" xr:uid="{453392DF-4A26-459E-991F-A450B5FF6FF9}"/>
+    <hyperlink ref="F33" tooltip="Manufacturer" display="'" xr:uid="{8C7E5E25-C237-4A0C-B57E-55B12EE06A8E}"/>
+    <hyperlink ref="I33" tooltip="Supplier" display="'" xr:uid="{AE83A388-CBF5-4675-8F4A-1E7A1A4F80EC}"/>
+    <hyperlink ref="F34" tooltip="Manufacturer" display="'" xr:uid="{2CC41660-A06D-4686-AA85-3C33BABFE9B8}"/>
+    <hyperlink ref="I34" tooltip="Supplier" display="'" xr:uid="{6F1AB5C3-0346-4A80-AC3E-E1D541CCF550}"/>
+    <hyperlink ref="F35" r:id="rId43" tooltip="Manufacturer" display="'RC0603FR-076K34L" xr:uid="{BF5EBF80-9E57-49C0-BB5D-1D8AC3EDFFF7}"/>
+    <hyperlink ref="I35" r:id="rId44" tooltip="Supplier" display="'311-6.34KHRDKR-ND" xr:uid="{5994FC85-C2FD-4427-A24F-BF9D3DFE7484}"/>
+    <hyperlink ref="F36" r:id="rId45" tooltip="Manufacturer" display="'RMCF0603FT698R" xr:uid="{34F510D4-0156-4E90-805A-366F764033A5}"/>
+    <hyperlink ref="I36" r:id="rId46" tooltip="Supplier" display="'RMCF0603FT698RDKR-ND" xr:uid="{3C5DBF7E-0504-4A93-AB62-9A92DE8A233C}"/>
+    <hyperlink ref="F37" tooltip="Manufacturer" display="'" xr:uid="{4F8D973D-6FFC-4F96-AEA9-B81392A788FF}"/>
+    <hyperlink ref="I37" tooltip="Supplier" display="'" xr:uid="{FB5FBFE2-F237-42C7-BB69-8247FF365620}"/>
+    <hyperlink ref="F38" r:id="rId47" tooltip="Manufacturer" display="'SS312SAH4-R" xr:uid="{69F9AEDD-A39A-430B-88A9-E5658D5B2E07}"/>
+    <hyperlink ref="I38" r:id="rId48" tooltip="Supplier" display="'360-2924-1-ND" xr:uid="{1840E8B3-B54B-4938-B369-7D1C4CF584AD}"/>
+    <hyperlink ref="F39" r:id="rId49" tooltip="Manufacturer" display="'TPS54383PWPR" xr:uid="{489617C5-17D8-4E63-9A6B-0B92288810D3}"/>
+    <hyperlink ref="I39" r:id="rId50" tooltip="Supplier" display="'296-23087-6-ND" xr:uid="{ADEF7E78-7E47-481B-921A-0E99C721888E}"/>
+    <hyperlink ref="F40" r:id="rId51" tooltip="Manufacturer" display="'INA199B2DCKR" xr:uid="{EE2CCB53-D986-476B-AAA1-7F022C6657D3}"/>
+    <hyperlink ref="I40" r:id="rId52" tooltip="Supplier" display="'INA199B2DCKR-ND" xr:uid="{306A7018-6508-4609-B485-9260D01DA30C}"/>
+    <hyperlink ref="F41" r:id="rId53" tooltip="Manufacturer" display="'TPS3705-33D" xr:uid="{74B32511-B38B-4ECA-96B0-12822E7C3461}"/>
+    <hyperlink ref="I41" r:id="rId54" tooltip="Supplier" display="'296-2623-5-ND" xr:uid="{5A1E294A-6F37-4CEA-82A2-831DB441B478}"/>
+    <hyperlink ref="F42" r:id="rId55" tooltip="Manufacturer" display="'LTC4365CTS8#TRMPBF" xr:uid="{75C5933B-7B9F-473B-AD65-4EAF0622803F}"/>
+    <hyperlink ref="I42" r:id="rId56" tooltip="Supplier" display="'LTC4365CTS8#TRMPBFDKR-ND" xr:uid="{278C8A56-C608-4C75-B084-A65FCBEF3D13}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId57"/>
+  <pageSetup orientation="portrait" r:id="rId57"/>
 </worksheet>
 </file>
</xml_diff>